<commit_message>
added ho chi minh
</commit_message>
<xml_diff>
--- a/Data/locations.xlsx
+++ b/Data/locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ayyanagouda\LCL Destination Charges Comparison Tool\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A72315CC-1619-4D15-8A83-68A02CBADAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D451C-D646-4E8A-9134-EF3FB7D8CD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{62138B79-7AA5-4A35-AB65-65B6655D184D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Hamburg</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>POD</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh City</t>
   </si>
 </sst>
 </file>
@@ -152,13 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,158 +494,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D1AE50-A142-4783-9FB8-7FE3DE7661BD}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>